<commit_message>
Add new testcase. Register with already registered email.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dilcorp-my.sharepoint.com/personal/rpecz_diligent_com/Documents/Desktop/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{CDE66FA6-103E-41C4-9FC9-FFC8FB30B26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9713F1B-AFA0-47F2-81DD-2769F6773E2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" r:id="rId1"/>
@@ -28,10 +27,10 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Login and register'!$B$1:$H$18</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -211,15 +210,30 @@
   <si>
     <t>Only if possible type password.</t>
   </si>
+  <si>
+    <t>001-10</t>
+  </si>
+  <si>
+    <t>Register user with email what is already registered</t>
+  </si>
+  <si>
+    <t>Use rob.pecz@gmail.com</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,19 +320,6 @@
       <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -481,14 +482,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,9 +577,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -587,12 +584,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -652,7 +648,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -934,7 +930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -942,8 +938,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1144,7 @@
       <c r="D3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="8">
@@ -1234,7 +1230,7 @@
     <row r="8" spans="1:156" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="17"/>
@@ -1285,6 +1281,10 @@
       <c r="H10" s="16" t="s">
         <v>4</v>
       </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1301,6 +1301,10 @@
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1317,6 +1321,10 @@
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1333,6 +1341,8 @@
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
       <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1349,6 +1359,8 @@
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
       <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1365,6 +1377,8 @@
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
       <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1381,8 +1395,10 @@
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="18" t="s">
         <v>45</v>
@@ -1397,8 +1413,10 @@
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
       <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="18" t="s">
         <v>46</v>
@@ -1413,8 +1431,10 @@
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
       <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="18" t="s">
         <v>51</v>
@@ -1431,17 +1451,29 @@
       <c r="H19" s="19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1451,7 +1483,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1461,7 +1493,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1471,7 +1503,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1481,7 +1513,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1491,7 +1523,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1501,7 +1533,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1511,7 +1543,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1521,7 +1553,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1531,7 +1563,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1541,7 +1573,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1551,7 +1583,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -10242,9 +10274,6 @@
       <c r="H900" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B20:H20"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D3">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="HIGH">
@@ -10258,7 +10287,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{0E402618-69C1-3F4A-8DD5-A3BFC67F08FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>$J$3:$J$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add new testcase. Register with already registered email. (#3)
Co-authored-by: Robert Pecz <rpecz-e@brainloop.com>
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dilcorp-my.sharepoint.com/personal/rpecz_diligent_com/Documents/Desktop/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{CDE66FA6-103E-41C4-9FC9-FFC8FB30B26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9713F1B-AFA0-47F2-81DD-2769F6773E2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" r:id="rId1"/>
@@ -28,10 +27,10 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Login and register'!$B$1:$H$18</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -211,15 +210,30 @@
   <si>
     <t>Only if possible type password.</t>
   </si>
+  <si>
+    <t>001-10</t>
+  </si>
+  <si>
+    <t>Register user with email what is already registered</t>
+  </si>
+  <si>
+    <t>Use rob.pecz@gmail.com</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,19 +320,6 @@
       <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -481,14 +482,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,9 +577,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -587,12 +584,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -652,7 +648,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -934,7 +930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -942,8 +938,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1144,7 @@
       <c r="D3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="8">
@@ -1234,7 +1230,7 @@
     <row r="8" spans="1:156" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="17"/>
@@ -1285,6 +1281,10 @@
       <c r="H10" s="16" t="s">
         <v>4</v>
       </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1301,6 +1301,10 @@
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1317,6 +1321,10 @@
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1333,6 +1341,8 @@
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
       <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1349,6 +1359,8 @@
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
       <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1365,6 +1377,8 @@
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
       <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1381,8 +1395,10 @@
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="18" t="s">
         <v>45</v>
@@ -1397,8 +1413,10 @@
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
       <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="18" t="s">
         <v>46</v>
@@ -1413,8 +1431,10 @@
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
       <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="18" t="s">
         <v>51</v>
@@ -1431,17 +1451,29 @@
       <c r="H19" s="19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1451,7 +1483,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1461,7 +1493,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1471,7 +1503,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1481,7 +1513,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1491,7 +1523,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1501,7 +1533,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1511,7 +1543,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1521,7 +1553,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1531,7 +1563,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1541,7 +1573,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1551,7 +1583,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -10242,9 +10274,6 @@
       <c r="H900" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B20:H20"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D3">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="HIGH">
@@ -10258,7 +10287,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{0E402618-69C1-3F4A-8DD5-A3BFC67F08FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>$J$3:$J$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add invalid email test. Fix execution errors.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dilcorp-my.sharepoint.com/personal/rpecz_diligent_com/Documents/Desktop/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{CDE66FA6-103E-41C4-9FC9-FFC8FB30B26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9713F1B-AFA0-47F2-81DD-2769F6773E2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" r:id="rId1"/>
@@ -28,10 +27,10 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Login and register'!$B$1:$H$18</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -211,15 +210,30 @@
   <si>
     <t>Only if possible type password.</t>
   </si>
+  <si>
+    <t>001-10</t>
+  </si>
+  <si>
+    <t>Register user with email what is already registered</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Use rob.pecz@gmail.com.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,19 +320,6 @@
       <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -481,12 +482,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -577,22 +577,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -652,7 +651,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -934,7 +933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -942,8 +941,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1147,7 @@
       <c r="D3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="8">
@@ -1193,7 +1192,9 @@
       <c r="E5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="27" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="28"/>
       <c r="H5" s="17"/>
       <c r="J5" s="24" t="s">
@@ -1285,6 +1286,10 @@
       <c r="H10" s="16" t="s">
         <v>4</v>
       </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1301,6 +1306,10 @@
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="33" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1317,6 +1326,10 @@
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="33" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1333,6 +1346,10 @@
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
       <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="33" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="14" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1349,6 +1366,8 @@
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
       <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1365,6 +1384,8 @@
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
       <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1381,8 +1402,10 @@
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="19"/>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="18" t="s">
         <v>45</v>
@@ -1397,8 +1420,10 @@
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
       <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="19"/>
+      <c r="J17" s="33"/>
+    </row>
+    <row r="18" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="18" t="s">
         <v>46</v>
@@ -1413,8 +1438,10 @@
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
       <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="19"/>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="18" t="s">
         <v>51</v>
@@ -1431,17 +1458,29 @@
       <c r="H19" s="19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I19" s="19"/>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="1:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1451,7 +1490,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1461,7 +1500,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1471,7 +1510,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1481,7 +1520,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1491,7 +1530,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1501,7 +1540,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1511,7 +1550,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1521,7 +1560,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1531,7 +1570,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1541,7 +1580,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1551,7 +1590,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -10242,9 +10281,6 @@
       <c r="H900" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B20:H20"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D3">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="HIGH">
@@ -10258,7 +10294,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{0E402618-69C1-3F4A-8DD5-A3BFC67F08FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>$J$3:$J$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add 001-04 Login with valid email and empty password testcase.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -938,8 +938,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1342,9 @@
       <c r="G13" s="21"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="J13" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1360,7 +1362,9 @@
       <c r="G14" s="21"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="J14" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
Add 001-04 Login with valid email and empty password testcase. (#5)
Co-authored-by: Robert Pecz <rpecz-e@brainloop.com>
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -938,8 +938,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1342,9 @@
       <c r="G13" s="21"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="J13" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1360,7 +1362,9 @@
       <c r="G14" s="21"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="J14" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:156" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
Add 001-06 register user with invalid email. Move errormessage into external static class.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="132">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -1198,9 +1198,9 @@
   </sheetPr>
   <dimension ref="A1:EZ900"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1670,10 +1670,14 @@
         <v>48</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -10654,8 +10658,8 @@
   </sheetPr>
   <dimension ref="A1:EZ900"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 001-06 register user with invalid email. Move errormessage into external static class. (#13)
Co-authored-by: Robert Pecz <rpecz-e@brainloop.com>
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="132">
   <si>
     <t>TEST DATE</t>
   </si>
@@ -1198,9 +1198,9 @@
   </sheetPr>
   <dimension ref="A1:EZ900"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1670,10 +1670,14 @@
         <v>48</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -10654,8 +10658,8 @@
   </sheetPr>
   <dimension ref="A1:EZ900"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement 15 register with invalid changed email testcase.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\CypressPetProject\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
   <si>
     <t>TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -1122,8 +1122,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1797,11 +1797,17 @@
       <c r="E24" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
+      <c r="F24" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="J24" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
@@ -1815,11 +1821,17 @@
       <c r="E25" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="J25" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>

</xml_diff>

<commit_message>
Register with invalid changed email testcase (#53)
Co-authored-by: Robert Pecz <rpecz-e@brainloop.com>
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\AutomationTest\CypressPetProject\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
   <si>
     <t>TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -1122,8 +1122,8 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1797,11 +1797,17 @@
       <c r="E24" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
+      <c r="F24" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="J24" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
@@ -1815,11 +1821,17 @@
       <c r="E25" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="J25" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>

</xml_diff>

<commit_message>
Add 001-17, 001-18, 001-19 testcases
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="133">
   <si>
     <t>TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -440,10 +440,10 @@
     <t>User shouldn't able to register without selecting date of birth month. Error message.</t>
   </si>
   <si>
-    <t>User shouldn't able to register without selecting date of birth year. Error message.</t>
+    <t>User should able to register without selecting date. Error message.</t>
   </si>
   <si>
-    <t>User should able to register without selecting date. Error message.</t>
+    <t xml:space="preserve">User should able to register without selecting date of birth year. </t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1845,11 +1845,17 @@
       <c r="E26" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
+      <c r="F26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H26" s="31"/>
       <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
+      <c r="J26" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
@@ -1863,11 +1869,17 @@
       <c r="E27" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="32"/>
+      <c r="F27" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="J27" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
@@ -1879,13 +1891,19 @@
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+        <v>132</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H28" s="31"/>
       <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="J28" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
@@ -1897,13 +1915,19 @@
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32"/>
+        <v>131</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H29" s="31"/>
       <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="J29" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>

</xml_diff>

<commit_message>
Register without select date of birth  (#55)
* Update automation_practice_testcases.xlsx.

* Delete unnecessary bool param. Add register without select dob day testcase.

* Add 001-17, 001-18, 001-19 testcases

---------

Co-authored-by: Robert Pecz <rpecz-e@brainloop.com>
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="133">
   <si>
     <t>TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -240,16 +240,10 @@
     <t>Register user without input first name.</t>
   </si>
   <si>
-    <t>User shouldn't able to register without input first name.</t>
-  </si>
-  <si>
     <t>001-13</t>
   </si>
   <si>
     <t>Register user without input last name.</t>
-  </si>
-  <si>
-    <t>User shouldn't able to register without input last name.</t>
   </si>
   <si>
     <t>001-14</t>
@@ -267,16 +261,7 @@
     <t>Register with invalid changed mail.</t>
   </si>
   <si>
-    <t>User shouldn't able to register with invalid change mail.</t>
-  </si>
-  <si>
     <t>001-16</t>
-  </si>
-  <si>
-    <t>Register without input password.</t>
-  </si>
-  <si>
-    <t>User shouldn't able to register without input password.</t>
   </si>
   <si>
     <t>001-17</t>
@@ -285,25 +270,13 @@
     <t>Register without select date of birth day.</t>
   </si>
   <si>
-    <t>User should able to register without selecting date of birth day.</t>
-  </si>
-  <si>
     <t>001-18</t>
   </si>
   <si>
     <t>Register without select date of birth month.</t>
   </si>
   <si>
-    <t>User should able to register without selecting date of birth month.</t>
-  </si>
-  <si>
-    <t>001-19</t>
-  </si>
-  <si>
     <t>Register without select date of birth year.</t>
-  </si>
-  <si>
-    <t>User should able to register without selecting date of birth year.</t>
   </si>
   <si>
     <t>Buy product</t>
@@ -444,6 +417,33 @@
   </si>
   <si>
     <t>User able to register.</t>
+  </si>
+  <si>
+    <t>001-19</t>
+  </si>
+  <si>
+    <t>Register without select.</t>
+  </si>
+  <si>
+    <t>User shouldn't able to register without input first name. Error message.</t>
+  </si>
+  <si>
+    <t>User shouldn't able to register without input last name. Error message.</t>
+  </si>
+  <si>
+    <t>User shouldn't able to register with invalid change mail. Error message.</t>
+  </si>
+  <si>
+    <t>User shouldn't able to register without selecting date of birth day. Error message.</t>
+  </si>
+  <si>
+    <t>User shouldn't able to register without selecting date of birth month. Error message.</t>
+  </si>
+  <si>
+    <t>User should able to register without selecting date. Error message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should able to register without selecting date of birth year. </t>
   </si>
 </sst>
 </file>
@@ -1119,11 +1119,11 @@
     <tabColor rgb="FF8497B0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EZ900"/>
+  <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1726,7 +1726,7 @@
         <v>62</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G21" s="32" t="s">
         <v>35</v>
@@ -1737,7 +1737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="29" t="s">
         <v>63</v>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="31" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>49</v>
@@ -1761,17 +1761,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="30" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>67</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="31" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>49</v>
@@ -1788,17 +1788,17 @@
     <row r="24" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>35</v>
@@ -1809,17 +1809,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="31" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>49</v>
@@ -1833,77 +1833,101 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
+        <v>129</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H26" s="31"/>
       <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
+      <c r="J26" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="32"/>
+        <v>130</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="J27" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="29" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+        <v>132</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H28" s="31"/>
       <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="J28" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="29" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32"/>
+        <v>131</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="H29" s="31"/>
       <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="J29" s="31" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
@@ -10604,16 +10628,6 @@
       <c r="F899" s="17"/>
       <c r="G899" s="17"/>
       <c r="H899" s="17"/>
-    </row>
-    <row r="900" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A900" s="17"/>
-      <c r="B900" s="17"/>
-      <c r="C900" s="17"/>
-      <c r="D900" s="17"/>
-      <c r="E900" s="17"/>
-      <c r="F900" s="17"/>
-      <c r="G900" s="17"/>
-      <c r="H900" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
@@ -10849,13 +10863,13 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F3" s="7">
         <v>14</v>
@@ -10891,7 +10905,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="19" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
@@ -10939,11 +10953,11 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="20" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="4"/>
@@ -10995,14 +11009,14 @@
     <row r="11" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="31" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="32" t="s">
@@ -11017,14 +11031,14 @@
     <row r="12" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="29" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="31" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="32"/>
@@ -11035,14 +11049,14 @@
     <row r="13" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="29" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="31" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="32"/>
@@ -11053,14 +11067,14 @@
     <row r="14" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="29" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="31" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="32"/>
@@ -11071,14 +11085,14 @@
     <row r="15" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="32"/>
@@ -11089,14 +11103,14 @@
     <row r="16" spans="1:156" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="29" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="31" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="32"/>
@@ -11107,14 +11121,14 @@
     <row r="17" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="29" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="31" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F17" s="33"/>
       <c r="G17" s="32"/>
@@ -11125,14 +11139,14 @@
     <row r="18" spans="1:10" ht="66" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="29" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="31" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="32"/>
@@ -11143,14 +11157,14 @@
     <row r="19" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="29" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="31" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F19" s="33"/>
       <c r="G19" s="32"/>
@@ -11161,14 +11175,14 @@
     <row r="20" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="29" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="31" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="32"/>
@@ -11178,14 +11192,14 @@
     </row>
     <row r="21" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="29" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="31" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="32"/>
@@ -11196,14 +11210,14 @@
     <row r="22" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="29" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="31" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="32"/>
@@ -11214,14 +11228,14 @@
     <row r="23" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="29" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="31" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="32"/>
@@ -11232,14 +11246,14 @@
     <row r="24" spans="1:10" ht="33" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="29" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="31" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="32"/>

</xml_diff>

<commit_message>
Implement add multiple product, remove one product. Update readme.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -364,6 +364,9 @@
     <t xml:space="preserve">Cart should be empty.</t>
   </si>
   <si>
+    <t xml:space="preserve">Cart empty after user deleting item from it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
@@ -371,6 +374,9 @@
   </si>
   <si>
     <t xml:space="preserve">Only that product is missing which is removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart has one product after other product is deleted.</t>
   </si>
   <si>
     <t xml:space="preserve">002-06</t>
@@ -605,7 +611,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.2497"/>
-        <bgColor rgb="FF333F50"/>
+        <bgColor rgb="FF333F4F"/>
       </patternFill>
     </fill>
     <fill>
@@ -1021,7 +1027,7 @@
       <rgbColor rgb="FF262626"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333F50"/>
+      <rgbColor rgb="FF333F4F"/>
       <rgbColor rgb="FF222A35"/>
     </indexedColors>
   </colors>
@@ -10754,9 +10760,9 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11183,41 +11189,53 @@
       <c r="E14" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="J14" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="33"/>
+        <v>110</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="J15" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="33"/>
@@ -11228,14 +11246,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11246,14 +11264,14 @@
     <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11264,14 +11282,14 @@
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11282,14 +11300,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11299,14 +11317,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11317,14 +11335,14 @@
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11335,14 +11353,14 @@
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11353,14 +11371,14 @@
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
33 002 05 add multiple product to the cart remove one product (#59)
* Minor fixes

* Implement add multiple product, remove one product. Update readme.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -364,6 +364,9 @@
     <t xml:space="preserve">Cart should be empty.</t>
   </si>
   <si>
+    <t xml:space="preserve">Cart empty after user deleting item from it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
@@ -371,6 +374,9 @@
   </si>
   <si>
     <t xml:space="preserve">Only that product is missing which is removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart has one product after other product is deleted.</t>
   </si>
   <si>
     <t xml:space="preserve">002-06</t>
@@ -605,7 +611,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.2497"/>
-        <bgColor rgb="FF333F50"/>
+        <bgColor rgb="FF333F4F"/>
       </patternFill>
     </fill>
     <fill>
@@ -1021,7 +1027,7 @@
       <rgbColor rgb="FF262626"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333F50"/>
+      <rgbColor rgb="FF333F4F"/>
       <rgbColor rgb="FF222A35"/>
     </indexedColors>
   </colors>
@@ -10754,9 +10760,9 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11183,41 +11189,53 @@
       <c r="E14" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="J14" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="33"/>
+        <v>110</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="J15" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="33"/>
@@ -11228,14 +11246,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11246,14 +11264,14 @@
     <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11264,14 +11282,14 @@
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11282,14 +11300,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11299,14 +11317,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11317,14 +11335,14 @@
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11335,14 +11353,14 @@
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11353,14 +11371,14 @@
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
Implement add one product and increased the size in the cart view. E2e.ts change back to .js
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart has increased the amount size.</t>
   </si>
   <si>
     <t xml:space="preserve">002-07</t>
@@ -10762,7 +10765,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11237,23 +11240,29 @@
       <c r="E16" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="J16" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11264,14 +11273,14 @@
     <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11282,14 +11291,14 @@
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11300,14 +11309,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11317,14 +11326,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11335,14 +11344,14 @@
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11353,14 +11362,14 @@
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11371,14 +11380,14 @@
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
34 002 06 add one product to the cart add more in the cart view (#60)
* Change viewport. Rename js files to ts.

* Implement add one product and increased the size in the cart view. E2e.ts change back to .js
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart has increased the amount size.</t>
   </si>
   <si>
     <t xml:space="preserve">002-07</t>
@@ -10762,7 +10765,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11237,23 +11240,29 @@
       <c r="E16" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="J16" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11264,14 +11273,14 @@
     <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11282,14 +11291,14 @@
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11300,14 +11309,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11317,14 +11326,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11335,14 +11344,14 @@
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11353,14 +11362,14 @@
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11371,14 +11380,14 @@
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>